<commit_message>
GrimWorld 40,000 - Framework - 3119805903 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/GrimWorld 40,000 - Framework - 3119805903/GrimWorld 40,000 - Framework - 3119805903.xlsx
+++ b/Data/GrimWorld 40,000 - Framework - 3119805903/GrimWorld 40,000 - Framework - 3119805903.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Data\haha\game\림월드 모드 번역\extractor 1.4\GrimWorld 40,000 - Framework - 3119805903\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SteamLibrary\steamapps\common\RimWorld\Mods\MOD KOREAN TRANSLATE\1.4\GrimWorld 40,000 - Framework - 3119805903\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FBC9C91-04FA-4D22-AFCC-6940E9E14257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF74DAFF-7508-4B57-9111-85A6ADFA90F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="88">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -256,6 +256,48 @@
   </si>
   <si>
     <t>{0}개 더</t>
+  </si>
+  <si>
+    <t>GW_FancyObelisk.label</t>
+  </si>
+  <si>
+    <t>GW_FancyObelisk.description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GW_OrdinaryObelisk.label</t>
+  </si>
+  <si>
+    <t>GW_OrdinaryObelisk.description</t>
+  </si>
+  <si>
+    <t>ThingDef</t>
+  </si>
+  <si>
+    <t>supporter monument center</t>
+  </si>
+  <si>
+    <t>A monument to those who helped make the GrimWorld project a reality.\n\n  Astartes tier:\n\nRainyredman1234, Bailey English\n\n  Primarch tier:\n\nFulgrim, R.CSN, kyle shadowchain, Echo\n\n  Emperor of Mankind tier:\n\nRisqué Che, Team Shibe</t>
+  </si>
+  <si>
+    <t>A monument to those who helped make the GrimWorld project a reality.\n\n  Servitor tier:\n\nAKorgar, Hell Fire, Sparrow, just a guy named brad\n\n  Guardsmen tier:\n\n♠_Caligula_♠, Józef Kozioł, MisterCroxo48\n\n  Stormtrooper tier:\n\nBenio, Alloyskull, Vylixan, Gofres, Celorico, Risque, Madgile\n\n  Neophyte tier:\n\nTacticalCrumpet, Petrie, JawnWick</t>
+  </si>
+  <si>
+    <t>supporter's monument</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>후원자 기념비</t>
+  </si>
+  <si>
+    <t>후원자 기념 센터</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그림월드 프로젝트의 실현을 도운 이들을 위한 기념비입니다.\n\n  아스타르테스 티어:\n\nRainyredman1234, Bailey English\n\n  프라이마크 티어:\n\nFulgrim, R.CSN, kyle shadowchain, Echo\n\n  인류의 황제 티어:\n\nRisqué Che, Team Shibe</t>
+  </si>
+  <si>
+    <t>그림월드 프로젝트의 실현을 도운 이들을 위한 기념비입니다.\n\n  서비터 티어:\n\nAKorgar, Hell Fire, Sparrow, just a guy named brad\n\n  가드맨 티어:\n\n♠_Caligula_♠, Józef Kozioł, MisterCroxo48\n\n  스톰트루퍼 티어:\n\nBenio, Alloyskull, Vylixan, Gofres, Celorico, Risque, Madgile\n\n  네오피테 티어:\n\nTacticalCrumpet, Petrie, JawnWick</t>
   </si>
 </sst>
 </file>
@@ -626,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -943,6 +985,62 @@
         <v>72</v>
       </c>
     </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" t="s">
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
GrimWorld 40,000 - Framework 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/GrimWorld 40,000 - Framework - 3119805903/GrimWorld 40,000 - Framework - 3119805903.xlsx
+++ b/Data/GrimWorld 40,000 - Framework - 3119805903/GrimWorld 40,000 - Framework - 3119805903.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SteamLibrary\steamapps\common\RimWorld\Mods\MOD KOREAN TRANSLATE\1.4\GrimWorld 40,000 - Framework - 3119805903\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SteamLibrary\steamapps\common\RimWorld\Mods\MOD KOREAN TRANSLATE\trans\GrimWorld 40,000 - Framework - 3119805903\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF74DAFF-7508-4B57-9111-85A6ADFA90F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA4F12A-11FD-4A91-BE81-C29190D123DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Lammergeier</author>
+  </authors>
+  <commentList>
+    <comment ref="D15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-04-21 이전의 원문: '{0} more'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-04-21에 새로 추가된 노드들 (11개)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="131">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -52,6 +88,9 @@
     <t>Missing at least one required gene.</t>
   </si>
   <si>
+    <t>필수 유전자가 하나 이상 누락되었습니다.</t>
+  </si>
+  <si>
     <t>pakageID</t>
   </si>
   <si>
@@ -64,6 +103,9 @@
     <t>Has none of required genes.</t>
   </si>
   <si>
+    <t>필수 유전자가 없습니다.</t>
+  </si>
+  <si>
     <t>Grimworld.Framework</t>
   </si>
   <si>
@@ -76,6 +118,32 @@
     <t>modName (folderName)</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Does not have the gene {0}.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>유전자 {0}(이)가 없습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Keyed+GW_GeneRestrictedEquipment_None</t>
   </si>
   <si>
@@ -85,6 +153,32 @@
     <t>GrimWorld 40,000 - Framework - 3119805903</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Has the gene {0}.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>유전자 {0}(을)를 가지고 있습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Keyed+GW_XenoRestrictedEquipment_AnyOne</t>
   </si>
   <si>
@@ -97,6 +191,19 @@
     <t>Keyed+GW_XenoRestrictedEquipment_One</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>필수 인종이 아닙니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>GW_XenoRestrictedEquipment_One</t>
   </si>
   <si>
@@ -106,6 +213,19 @@
     <t>Keyed+GW_XenoRestrictedEquipment_None</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{0}(이)가 아닙니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>GW_XenoRestrictedEquipment_None</t>
   </si>
   <si>
@@ -115,12 +235,28 @@
     <t>Keyed+GW_GenesNotFound</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{0} 입니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>GW_GenesNotFound</t>
   </si>
   <si>
     <t>Genes are required to equip this item.</t>
   </si>
   <si>
+    <t>이 아이템을 장착하려면 유전자가 필요합니다.</t>
+  </si>
+  <si>
     <t>Keyed+GW_HediffRestrictedEquipment_All</t>
   </si>
   <si>
@@ -130,6 +266,9 @@
     <t>Missing at least one required hediff.</t>
   </si>
   <si>
+    <t>하나 이상의 필수 헤디프가 누락되었습니다.</t>
+  </si>
+  <si>
     <t>Keyed+GW_HediffRestrictedEquipment_AnyOne</t>
   </si>
   <si>
@@ -139,6 +278,9 @@
     <t>Has none of required hediffs.</t>
   </si>
   <si>
+    <t>필수 헤디프가 없습니다.</t>
+  </si>
+  <si>
     <t>Keyed+GW_HediffRestrictedEquipment_One</t>
   </si>
   <si>
@@ -151,6 +293,19 @@
     <t>Keyed+GW_HediffRestrictedEquipment_None</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>헤디프 {0}(이)가 없습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>GW_HediffRestrictedEquipment_None</t>
   </si>
   <si>
@@ -160,6 +315,19 @@
     <t>Keyed+GW_RequiresStudyOf</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>헤디프 {0}(이)가 있습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>GW_RequiresStudyOf</t>
   </si>
   <si>
@@ -169,10 +337,26 @@
     <t>Keyed+GW_MoreNeeded</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>학습 필요:</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>GW_MoreNeeded</t>
   </si>
   <si>
-    <t>{0} more</t>
+    <t>JobDef+CarryToIndoctrinatingChamberJob.reportString</t>
+  </si>
+  <si>
+    <t>{0}개 더</t>
   </si>
   <si>
     <t>Keyed+GW_StudyAt</t>
@@ -187,124 +371,234 @@
     <t>Keyed+GW_DiscoveredResearch</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{0}에서</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>GW_DiscoveredResearch</t>
   </si>
   <si>
     <t>You've discovered this research.</t>
   </si>
   <si>
-    <t>필수 유전자가 하나 이상 누락되었습니다.</t>
-  </si>
-  <si>
-    <t>필수 유전자가 없습니다.</t>
-  </si>
-  <si>
-    <t>Does not have the gene {0}.</t>
+    <t>이 연구를 발견했습니다.</t>
+  </si>
+  <si>
+    <t>ThingDef</t>
+  </si>
+  <si>
+    <t>GW_FancyObelisk.label</t>
+  </si>
+  <si>
+    <t>supporter monument center</t>
+  </si>
+  <si>
+    <t>A monument to those who helped make the GrimWorld project a reality.\n\n  Astartes tier:\n\nRainyredman1234, Bailey English\n\n  Primarch tier:\n\nFulgrim, R.CSN, kyle shadowchain, Echo\n\n  Emperor of Mankind tier:\n\nRisqué Che, Team Shibe</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>후원자 기념 센터</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GW_FancyObelisk.description</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>그림월드 프로젝트의 실현을 도운 이들을 위한 기념비입니다.\n\n  아스타르테스 티어:\n\nRainyredman1234, Bailey English\n\n  프라이마크 티어:\n\nFulgrim, R.CSN, kyle shadowchain, Echo\n\n  인류의 황제 티어:\n\nRisqué Che, Team Shibe</t>
+  </si>
+  <si>
+    <t>GW_OrdinaryObelisk.label</t>
+  </si>
+  <si>
+    <t>후원자 기념비</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>supporter's monument</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>GW_OrdinaryObelisk.description</t>
+  </si>
+  <si>
+    <t>A monument to those who helped make the GrimWorld project a reality.\n\n  Servitor tier:\n\nAKorgar, Hell Fire, Sparrow, just a guy named brad\n\n  Guardsmen tier:\n\n♠_Caligula_♠, Józef Kozioł, MisterCroxo48\n\n  Stormtrooper tier:\n\nBenio, Alloyskull, Vylixan, Gofres, Celorico, Risque, Madgile\n\n  Neophyte tier:\n\nTacticalCrumpet, Petrie, JawnWick</t>
+  </si>
+  <si>
+    <t>그림월드 프로젝트의 실현을 도운 이들을 위한 기념비입니다.\n\n  서비터 티어:\n\nAKorgar, Hell Fire, Sparrow, just a guy named brad\n\n  가드맨 티어:\n\n♠_Caligula_♠, Józef Kozioł, MisterCroxo48\n\n  스톰트루퍼 티어:\n\nBenio, Alloyskull, Vylixan, Gofres, Celorico, Risque, Madgile\n\n  네오피테 티어:\n\nTacticalCrumpet, Petrie, JawnWick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{0} more </t>
+  </si>
+  <si>
+    <t>JobDef</t>
+  </si>
+  <si>
+    <t>CarryToIndoctrinatingChamberJob.reportString</t>
+  </si>
+  <si>
+    <t>carrying TargetA to indoctrinating chamber.</t>
+  </si>
+  <si>
+    <t>HediffDef+IndoctrinationChamber_BrainDamage.labelNounPretty</t>
+  </si>
+  <si>
+    <t>HediffDef</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamber_BrainDamage.labelNounPretty</t>
+  </si>
+  <si>
+    <t>{0} in the {1}</t>
+  </si>
+  <si>
+    <t>HediffDef+IndoctrinationChamber_BrainDamage.label</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamber_BrainDamage.label</t>
+  </si>
+  <si>
+    <t>brainwash damage</t>
+  </si>
+  <si>
+    <t>HediffDef+IndoctrinationChamber_BrainDamage.labelNoun</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamber_BrainDamage.labelNoun</t>
+  </si>
+  <si>
+    <t>HediffDef+IndoctrinationChamber_BrainDamage.description</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamber_BrainDamage.description</t>
+  </si>
+  <si>
+    <t>Brainwash Damage.</t>
+  </si>
+  <si>
+    <t>HediffDef+IndoctrinationChamber_BrainDamage.injuryProps.destroyedLabel</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamber_BrainDamage.injuryProps.destroyedLabel</t>
+  </si>
+  <si>
+    <t>Torn off</t>
+  </si>
+  <si>
+    <t>HediffDef+IndoctrinationChamber_BrainDamage.injuryProps.destroyedOutLabel</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamber_BrainDamage.injuryProps.destroyedOutLabel</t>
+  </si>
+  <si>
+    <t>Torn out</t>
+  </si>
+  <si>
+    <t>HediffDef+IndoctrinationChamber_BrainDamage.comps.0.permanentLabel</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamber_BrainDamage.comps.0.permanentLabel</t>
+  </si>
+  <si>
+    <t>brainwashed</t>
+  </si>
+  <si>
+    <t>HediffDef+IndoctrinationChamberSickness.label</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamberSickness.label</t>
+  </si>
+  <si>
+    <t>indoctrination chamber sickness</t>
+  </si>
+  <si>
+    <t>HediffDef+IndoctrinationChamberSickness.description</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamberSickness.description</t>
+  </si>
+  <si>
+    <t>placeholder.</t>
+  </si>
+  <si>
+    <t>HediffDef+IndoctrinationChamberSickness.descriptionShort</t>
+  </si>
+  <si>
+    <t>IndoctrinationChamberSickness.descriptionShort</t>
+  </si>
+  <si>
+    <t>After-effects of using a cryptosleep pod including dizziness, nausea, and vomiting.</t>
+  </si>
+  <si>
+    <t>TargetA(을)를 세뇌실로 옮깁니다.</t>
+  </si>
+  <si>
+    <t>{1}의 {0}</t>
+  </si>
+  <si>
+    <t>세뇌 손상</t>
+  </si>
+  <si>
+    <t>찢어짐</t>
+  </si>
+  <si>
+    <t>뜯음</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>유전자 {0}(이)가 없습니다.</t>
+    <t>세뇌됨</t>
+  </si>
+  <si>
+    <t>세뇌실병</t>
+  </si>
+  <si>
+    <t>어지러움, 메스꺼움, 구토 등 동면관 사용 후유증이 발생할 수 있습니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Has the gene {0}.</t>
+    <t>플레이스홀더.</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>유전자 {0}(을)를 가지고 있습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>필수 인종이 아닙니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{0}(이)가 아닙니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{0} 입니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이 아이템을 장착하려면 유전자가 필요합니다.</t>
-  </si>
-  <si>
-    <t>하나 이상의 필수 헤디프가 누락되었습니다.</t>
-  </si>
-  <si>
-    <t>필수 헤디프가 없습니다.</t>
-  </si>
-  <si>
-    <t>헤디프 {0}(이)가 없습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>헤디프 {0}(이)가 있습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>학습 필요:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이 연구를 발견했습니다.</t>
-  </si>
-  <si>
-    <t>{0}에서</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{0}개 더</t>
-  </si>
-  <si>
-    <t>GW_FancyObelisk.label</t>
-  </si>
-  <si>
-    <t>GW_FancyObelisk.description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GW_OrdinaryObelisk.label</t>
-  </si>
-  <si>
-    <t>GW_OrdinaryObelisk.description</t>
-  </si>
-  <si>
-    <t>ThingDef</t>
-  </si>
-  <si>
-    <t>supporter monument center</t>
-  </si>
-  <si>
-    <t>A monument to those who helped make the GrimWorld project a reality.\n\n  Astartes tier:\n\nRainyredman1234, Bailey English\n\n  Primarch tier:\n\nFulgrim, R.CSN, kyle shadowchain, Echo\n\n  Emperor of Mankind tier:\n\nRisqué Che, Team Shibe</t>
-  </si>
-  <si>
-    <t>A monument to those who helped make the GrimWorld project a reality.\n\n  Servitor tier:\n\nAKorgar, Hell Fire, Sparrow, just a guy named brad\n\n  Guardsmen tier:\n\n♠_Caligula_♠, Józef Kozioł, MisterCroxo48\n\n  Stormtrooper tier:\n\nBenio, Alloyskull, Vylixan, Gofres, Celorico, Risque, Madgile\n\n  Neophyte tier:\n\nTacticalCrumpet, Petrie, JawnWick</t>
-  </si>
-  <si>
-    <t>supporter's monument</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>후원자 기념비</t>
-  </si>
-  <si>
-    <t>후원자 기념 센터</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그림월드 프로젝트의 실현을 도운 이들을 위한 기념비입니다.\n\n  아스타르테스 티어:\n\nRainyredman1234, Bailey English\n\n  프라이마크 티어:\n\nFulgrim, R.CSN, kyle shadowchain, Echo\n\n  인류의 황제 티어:\n\nRisqué Che, Team Shibe</t>
-  </si>
-  <si>
-    <t>그림월드 프로젝트의 실현을 도운 이들을 위한 기념비입니다.\n\n  서비터 티어:\n\nAKorgar, Hell Fire, Sparrow, just a guy named brad\n\n  가드맨 티어:\n\n♠_Caligula_♠, Józef Kozioł, MisterCroxo48\n\n  스톰트루퍼 티어:\n\nBenio, Alloyskull, Vylixan, Gofres, Celorico, Risque, Madgile\n\n  네오피테 티어:\n\nTacticalCrumpet, Petrie, JawnWick</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -319,8 +613,14 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -347,6 +647,16 @@
         <fgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF87CEEB"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -360,12 +670,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -667,18 +979,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="37" customWidth="1"/>
+    <col min="1" max="2" width="9.125" customWidth="1"/>
+    <col min="3" max="3" width="45.375" customWidth="1"/>
     <col min="4" max="4" width="42.125" customWidth="1"/>
     <col min="5" max="5" width="34.625" customWidth="1"/>
+    <col min="6" max="6" width="9.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -715,335 +1029,523 @@
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>58</v>
+        <v>15</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>50</v>
+        <v>64</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" t="s">
         <v>79</v>
-      </c>
-      <c r="C18" t="s">
-        <v>75</v>
-      </c>
-      <c r="D18" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C19" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D19" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" t="s">
         <v>81</v>
-      </c>
-      <c r="E19" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" t="s">
         <v>83</v>
-      </c>
-      <c r="E20" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C21" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="D21" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E21" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E23" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" t="s">
+        <v>95</v>
+      </c>
+      <c r="E24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" t="s">
+        <v>98</v>
+      </c>
+      <c r="E25" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" t="s">
+        <v>98</v>
+      </c>
+      <c r="E26" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>104</v>
+      </c>
+      <c r="B28" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" t="s">
+        <v>105</v>
+      </c>
+      <c r="D28" t="s">
+        <v>106</v>
+      </c>
+      <c r="E28" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" t="s">
+        <v>108</v>
+      </c>
+      <c r="D29" t="s">
+        <v>109</v>
+      </c>
+      <c r="E29" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" t="s">
+        <v>112</v>
+      </c>
+      <c r="E30" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" t="s">
+        <v>114</v>
+      </c>
+      <c r="D31" t="s">
+        <v>115</v>
+      </c>
+      <c r="E31" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>116</v>
+      </c>
+      <c r="B32" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" t="s">
+        <v>117</v>
+      </c>
+      <c r="D32" t="s">
+        <v>118</v>
+      </c>
+      <c r="E32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>119</v>
+      </c>
+      <c r="B33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" t="s">
+        <v>120</v>
+      </c>
+      <c r="D33" t="s">
+        <v>121</v>
+      </c>
+      <c r="E33" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>